<commit_message>
Adding Readme and improving gameplay
</commit_message>
<xml_diff>
--- a/Diagram.xlsx
+++ b/Diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\C#\BattleshipGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0B84046-B0B0-463B-8DDC-B24459C879EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE150E2B-74DF-4A43-BD9E-BDDC07BB5B63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="0" windowWidth="21864" windowHeight="9660" xr2:uid="{18B28CFD-E091-4DD4-9DDB-9AB93420C0DA}"/>
+    <workbookView xWindow="3528" yWindow="0" windowWidth="21864" windowHeight="9660" xr2:uid="{18B28CFD-E091-4DD4-9DDB-9AB93420C0DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +158,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -413,11 +407,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -434,20 +425,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,7 +756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6560A7C-9E1B-4BF8-AD5E-07C474586349}">
   <dimension ref="B1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -775,446 +769,446 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>2</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>3</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>4</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>5</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>6</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>7</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <v>8</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="18"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2">
         <v>14</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="15">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="14">
         <v>18</v>
       </c>
-      <c r="L4" s="18"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="18"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="17">
         <v>30</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="18"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="18"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="11"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="5">
+      <c r="C9" s="1"/>
+      <c r="D9" s="4">
         <v>61</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="6">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="5">
         <v>66</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="11"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="11"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="11"/>
-      <c r="N11" s="22" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="10"/>
+      <c r="N11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="22" t="s">
+      <c r="O11" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-      <c r="N12" s="28" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+      <c r="N12" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="N13" s="27" t="s">
+      <c r="N13" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="N14" s="26" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="N14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N15" s="24" t="s">
+      <c r="N15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7">
         <v>0</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>3</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>4</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>5</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>6</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="7">
         <v>7</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="7">
         <v>8</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="8">
         <v>9</v>
       </c>
-      <c r="N16" s="21" t="s">
+      <c r="N16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>0</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="11"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>1</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="11"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="10"/>
     </row>
     <row r="19" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>2</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="11"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>3</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="15">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="14">
         <v>35</v>
       </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="17"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="16"/>
     </row>
     <row r="21" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>4</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="5">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="4">
         <v>43</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="11"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>5</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="11"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="10"/>
     </row>
     <row r="23" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>6</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>60</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="6">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="5">
         <v>65</v>
       </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="11"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="10"/>
     </row>
     <row r="24" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>7</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="16">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="15">
         <v>73</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="11"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="10"/>
     </row>
     <row r="25" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>8</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="11"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="10"/>
     </row>
     <row r="26" spans="2:12" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="12">
+      <c r="B26" s="11">
         <v>9</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="13"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update sample design layout
</commit_message>
<xml_diff>
--- a/Diagram.xlsx
+++ b/Diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\C#\BattleshipGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE150E2B-74DF-4A43-BD9E-BDDC07BB5B63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{83E6B6F8-2A0E-4676-B279-FAD2C7B57F8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3528" yWindow="0" windowWidth="21864" windowHeight="9660" xr2:uid="{18B28CFD-E091-4DD4-9DDB-9AB93420C0DA}"/>
+    <workbookView xWindow="5880" yWindow="0" windowWidth="21864" windowHeight="9660" xr2:uid="{18B28CFD-E091-4DD4-9DDB-9AB93420C0DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,13 +70,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,12 +116,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,13 +394,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -423,23 +409,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,7 +743,7 @@
   <dimension ref="B1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,40 +755,40 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6"/>
-      <c r="C2" s="7">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>2</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>3</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>4</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>5</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>6</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <v>7</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>8</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
@@ -814,10 +800,10 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
@@ -830,60 +816,74 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>18</v>
       </c>
-      <c r="L4" s="10"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>24</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="10"/>
+      <c r="K5" s="13">
+        <v>28</v>
+      </c>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="26">
         <v>30</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="26">
+        <v>31</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>34</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="10"/>
+      <c r="K6" s="13">
+        <v>38</v>
+      </c>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <v>44</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="10"/>
+      <c r="K7" s="13">
+        <v>48</v>
+      </c>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>5</v>
       </c>
       <c r="C8" s="1"/>
@@ -894,30 +894,40 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="10"/>
+      <c r="K8" s="13">
+        <v>58</v>
+      </c>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" spans="2:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>6</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>61</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="3">
+        <v>62</v>
+      </c>
+      <c r="F9" s="3">
+        <v>63</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>66</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="10"/>
+      <c r="J9" s="4">
+        <v>67</v>
+      </c>
+      <c r="K9" s="4">
+        <v>68</v>
+      </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>7</v>
       </c>
       <c r="C10" s="1"/>
@@ -929,10 +939,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="10"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>8</v>
       </c>
       <c r="C11" s="1"/>
@@ -944,106 +954,106 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="10"/>
-      <c r="N11" s="19" t="s">
+      <c r="L11" s="9"/>
+      <c r="N11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="O11" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>9</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="N12" s="25" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+      <c r="N12" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="24">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="N14" s="23" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="N14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6">
         <v>0</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>3</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>4</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>5</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>6</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>7</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>8</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="7">
         <v>9</v>
       </c>
-      <c r="N16" s="18" t="s">
+      <c r="N16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>0</v>
       </c>
       <c r="C17" s="1"/>
@@ -1055,10 +1065,10 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>1</v>
       </c>
       <c r="C18" s="1"/>
@@ -1070,10 +1080,10 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="10"/>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>2</v>
       </c>
       <c r="C19" s="1"/>
@@ -1085,10 +1095,10 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="10"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>3</v>
       </c>
       <c r="C20" s="1"/>
@@ -1096,33 +1106,33 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>35</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="16"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="9">
+      <c r="B21" s="8">
         <v>4</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>43</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="10"/>
+      <c r="L21" s="9"/>
     </row>
     <row r="22" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="9">
+      <c r="B22" s="8">
         <v>5</v>
       </c>
       <c r="C22" s="1"/>
@@ -1134,10 +1144,10 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="10"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="9">
+      <c r="B23" s="8">
         <v>6</v>
       </c>
       <c r="C23" s="2">
@@ -1147,33 +1157,33 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>65</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="10"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>7</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <v>73</v>
       </c>
-      <c r="G24" s="15"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="10"/>
+      <c r="L24" s="9"/>
     </row>
     <row r="25" spans="2:12" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>8</v>
       </c>
       <c r="C25" s="1"/>
@@ -1185,30 +1195,30 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="10"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="26" spans="2:12" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>9</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>